<commit_message>
Delete deprecated InitializingProjectListener and InitializingModuleListener
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.project/test/resources/multi-module-support/test1/project1/Module1_1.xlsx
+++ b/STUDIO/org.openl.rules.project/test/resources/multi-module-support/test1/project1/Module1_1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="285" yWindow="105" windowWidth="16140" windowHeight="9210"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>C1</t>
   </si>
@@ -67,16 +67,31 @@
   </si>
   <si>
     <t>Standard Risk Driver</t>
+  </si>
+  <si>
+    <t>scope</t>
+  </si>
+  <si>
+    <t>lob</t>
+  </si>
+  <si>
+    <t>lob1</t>
+  </si>
+  <si>
+    <t>Properties moduleProperties</t>
+  </si>
+  <si>
+    <t>Module</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -350,12 +365,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -384,44 +432,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -429,11 +444,16 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Vehicle-Eligibility"/>
@@ -833,14 +853,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A4:I11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.85546875" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="9.85546875" customWidth="1" collapsed="1"/>
@@ -852,102 +872,117 @@
     <col min="9" max="9" width="21.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:7">
-      <c r="C4" s="19" t="s">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="21"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="3:7">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="23"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="3:7">
-      <c r="C6" s="24" t="s">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C6" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25" t="s">
+      <c r="D6" s="9"/>
+      <c r="E6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="25"/>
-      <c r="G6" s="26"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="3:7">
-      <c r="C7" s="27" t="s">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28" t="s">
+      <c r="D7" s="12"/>
+      <c r="E7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="28"/>
-      <c r="G7" s="29"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="13"/>
     </row>
-    <row r="8" spans="3:7">
-      <c r="C8" s="7" t="s">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C8" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="9" t="s">
+      <c r="D8" s="19"/>
+      <c r="E8" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="10"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
     </row>
-    <row r="9" spans="3:7">
-      <c r="C9" s="11" t="s">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C9" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="13" t="s">
+      <c r="D9" s="23"/>
+      <c r="E9" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="14"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="25"/>
     </row>
-    <row r="10" spans="3:7">
-      <c r="C10" s="15" t="s">
+    <row r="10" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C10" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="17">
+      <c r="D10" s="27"/>
+      <c r="E10" s="28">
         <v>100</v>
       </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="18"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="29"/>
     </row>
-    <row r="11" spans="3:7">
-      <c r="C11" s="3" t="s">
+    <row r="11" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="5">
+      <c r="D11" s="15"/>
+      <c r="E11" s="16">
         <v>5</v>
       </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="6"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="17"/>
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:G7"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="C8:D8"/>
@@ -956,6 +991,12 @@
     <mergeCell ref="E9:G9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="E10:G10"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:G7"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>